<commit_message>
updated biolog mapping to coralme
</commit_message>
<xml_diff>
--- a/species_files/Zymomonas_mobilis/verification_data/biolog_10_1016_j_synbio_2023_07_001.xlsx
+++ b/species_files/Zymomonas_mobilis/verification_data/biolog_10_1016_j_synbio_2023_07_001.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cdall/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cdall/github/coralme/species_files/Zymomonas_mobilis/verification_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31EDD51B-4A4F-314D-B823-599F596956B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97C0923-8ED1-A44F-928F-DCCF9513C87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{1B5CB503-34FF-514A-A2AB-61A120CB47CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2660" uniqueCount="1277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2661" uniqueCount="1278">
   <si>
     <t>PM_ID</t>
   </si>
@@ -3867,6 +3867,9 @@
   </si>
   <si>
     <t>iZM4_478 prediction</t>
+  </si>
+  <si>
+    <t>ID in coralme</t>
   </si>
 </sst>
 </file>
@@ -3928,13 +3931,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4271,10 +4274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232C9AB5-46F7-5B41-9464-8F1ADDB49267}">
-  <dimension ref="A1:G380"/>
+  <dimension ref="A1:H380"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4286,7 +4289,7 @@
     <col min="7" max="7" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4308,8 +4311,11 @@
       <c r="G1" s="4" t="s">
         <v>1276</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="2" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -4332,7 +4338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -4355,7 +4361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -4378,7 +4384,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -4401,7 +4407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -4424,7 +4430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -4447,7 +4453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -4470,7 +4476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -4493,7 +4499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -4516,7 +4522,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
@@ -4539,7 +4545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
@@ -4562,7 +4568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
@@ -4585,7 +4591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -4608,7 +4614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
@@ -4631,7 +4637,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>63</v>
       </c>

</xml_diff>